<commit_message>
Ajout de la BDD salle -> Mise en place BDD/Page de listing/Relation avec Manifs
</commit_message>
<xml_diff>
--- a/ressources/data.xlsx
+++ b/ressources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bende\Docker\www\SAE301\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA00DD60-D794-486A-A923-0167F758D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B99A2F-769F-4D09-B1AB-07EA87E0BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3887E5D8-3EDB-4C1D-AE3B-F4A53032B9AB}"/>
+    <workbookView xWindow="-4095" yWindow="3570" windowWidth="9000" windowHeight="7875" xr2:uid="{3887E5D8-3EDB-4C1D-AE3B-F4A53032B9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -602,82 +602,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1005,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C486D1AC-F30A-4FC1-B0F1-775E47FCC621}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="68" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,12 +1013,12 @@
     <col min="6" max="6" width="57.42578125" style="4" customWidth="1"/>
     <col min="7" max="8" width="11.42578125" style="4"/>
     <col min="9" max="9" width="23.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="168.85546875" style="24" customWidth="1"/>
-    <col min="11" max="11" width="55.28515625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="55.28515625" style="28" customWidth="1"/>
-    <col min="13" max="13" width="55.28515625" style="24" customWidth="1"/>
+    <col min="10" max="10" width="168.85546875" style="23" customWidth="1"/>
+    <col min="11" max="11" width="55.28515625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="55.28515625" style="26" customWidth="1"/>
+    <col min="13" max="13" width="55.28515625" style="23" customWidth="1"/>
     <col min="14" max="15" width="11.42578125" style="4"/>
-    <col min="16" max="16" width="110.28515625" style="25" customWidth="1"/>
+    <col min="16" max="16" width="110.28515625" style="4" customWidth="1"/>
     <col min="17" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
@@ -1056,7 +1050,7 @@
       <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="27"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="6"/>
       <c r="N1" s="5" t="s">
         <v>12</v>
@@ -1064,785 +1058,785 @@
       <c r="O1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="E2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>1088</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="1">
         <v>44948</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9">
         <v>25</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>502</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="1">
         <v>44932</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <v>20</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>102</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="1">
         <v>44935</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <v>25</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>100</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="1">
         <v>44941</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>20</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>130</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="1">
         <v>44942</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>25</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="10" t="s">
         <v>92</v>
       </c>
       <c r="L7" s="1">
         <v>44976</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>5</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="P7" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="I8" s="10" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="I8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="1">
         <v>44928</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>5</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>38</v>
       </c>
       <c r="L9" s="1">
         <v>44927</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>5</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="P9" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="180" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>45</v>
       </c>
       <c r="L10" s="1">
         <v>44949</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>12</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>91</v>
       </c>
       <c r="L11" s="1">
         <v>44951</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>26</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="P11" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="10" t="s">
         <v>52</v>
       </c>
       <c r="L12" s="1">
         <v>44953</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>20</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="P12" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="10" t="s">
         <v>55</v>
       </c>
       <c r="L13" s="1">
         <v>44943</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>5</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P13" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="I14" s="10" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="I14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>89</v>
       </c>
       <c r="L14" s="1">
         <v>44966</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>22</v>
       </c>
-      <c r="P14" s="12" t="s">
+      <c r="P14" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="10" t="s">
         <v>88</v>
       </c>
       <c r="L15" s="1">
         <v>44934</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="N15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>25</v>
       </c>
-      <c r="P15" s="12" t="s">
+      <c r="P15" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="10" t="s">
         <v>65</v>
       </c>
       <c r="L16" s="1">
         <v>44978</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="N16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>5</v>
       </c>
-      <c r="P16" s="12" t="s">
+      <c r="P16" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="10" t="s">
         <v>69</v>
       </c>
       <c r="L17" s="1">
         <v>44951</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="N17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9">
         <v>23</v>
       </c>
-      <c r="P17" s="12" t="s">
+      <c r="P17" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="10" t="s">
         <v>90</v>
       </c>
       <c r="L18" s="1">
         <v>44975</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="9">
         <v>5</v>
       </c>
-      <c r="P18" s="12" t="s">
+      <c r="P18" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="10" t="s">
         <v>74</v>
       </c>
       <c r="L19" s="1">
         <v>44930</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="9">
         <v>8</v>
       </c>
-      <c r="P19" s="12" t="s">
+      <c r="P19" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="I20" s="10" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="I20" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="10" t="s">
         <v>77</v>
       </c>
       <c r="L20" s="1">
         <v>44956</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>20</v>
       </c>
-      <c r="P20" s="12" t="s">
+      <c r="P20" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="10" t="s">
         <v>80</v>
       </c>
       <c r="L21" s="1">
         <v>44927</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="10" t="s">
+      <c r="N21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>25</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="P21" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="24" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>